<commit_message>
Final update from the NBA season.
</commit_message>
<xml_diff>
--- a/Win Formatting.xlsx
+++ b/Win Formatting.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10700" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11660" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="127">
   <si>
     <t>Arizona Cardinals</t>
   </si>
@@ -408,13 +408,25 @@
   </si>
   <si>
     <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Season End</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Finals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -442,6 +454,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +499,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -689,8 +709,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,8 +743,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -815,6 +852,14 @@
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -917,6 +962,14 @@
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4464,10 +4517,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="V1" activePane="topRight" state="frozenSplit"/>
+      <pane xSplit="4" topLeftCell="AA1" activePane="topRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
@@ -4481,7 +4534,7 @@
     <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="16" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -4500,7 +4553,7 @@
         <v>42678</v>
       </c>
       <c r="G1" s="8">
-        <f t="shared" ref="G1:Z1" si="0">F1+7</f>
+        <f t="shared" ref="G1:Y1" si="0">F1+7</f>
         <v>42685</v>
       </c>
       <c r="H1" s="8">
@@ -4572,11 +4625,26 @@
       <c r="Z1" s="8">
         <v>42821</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AA1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" s="2" t="str">
-        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,",",$K2,",",$L2,",",$M2,",",$N2,",",$O2,",",$P2,",",$Q2,",",$R2,",",$S2,",",$T2,",",$U2,",",$V2,",",$W2,",",$X2,",",$Y2,",",$Z2,"],")</f>
-        <v>['Zach', 'Atlanta' ,1,3,6,9,10,10,12,13,15,17,20,23,25,27,29,31,32,32,34,36,37,37],</v>
+        <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,",",$K2,",",$L2,",",$M2,",",$N2,",",$O2,",",$P2,",",$Q2,",",$R2,",",$S2,",",$T2,",",$U2,",",$V2,",",$W2,",",$X2,",",$Y2,",",$Z2,",",$AA2,",",$AB2,",",$AC2,"],")</f>
+        <v>['Zach', 'Atlanta' ,1,3,6,9,10,10,12,13,15,17,20,23,25,27,29,31,32,32,34,36,37,37,43,45,45],</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
@@ -4651,11 +4719,26 @@
       <c r="Z2">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="AA2">
+        <v>43</v>
+      </c>
+      <c r="AB2">
+        <v>45</v>
+      </c>
+      <c r="AC2">
+        <v>45</v>
+      </c>
+      <c r="AD2">
+        <v>45</v>
+      </c>
+      <c r="AE2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" s="2" t="str">
-        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,",",$U3,",",$V3,",",$W3,",",$X3,",",$Y3,",",$Z3,"],")</f>
-        <v>['Jeff', 'Boston' ,1,3,4,6,9,11,13,14,17,20,22,25,26,28,32,34,37,37,40,41,44,48],</v>
+        <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,",",$U3,",",$V3,",",$W3,",",$X3,",",$Y3,",",$Z3,",",$AA3,",",$AB3,",",$AC3,"],")</f>
+        <v>['Jeff', 'Boston' ,1,3,4,6,9,11,13,14,17,20,22,25,26,28,32,34,37,37,40,41,44,48,53,57,61],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -4730,11 +4813,20 @@
       <c r="Z3">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="AA3">
+        <v>53</v>
+      </c>
+      <c r="AB3">
+        <v>57</v>
+      </c>
+      <c r="AC3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Brooklyn' ,1,2,3,4,4,5,6,7,7,8,8,8,9,9,9,9,9,9,10,11,13,16],</v>
+        <v>['Zach', 'Brooklyn' ,1,2,3,4,4,5,6,7,7,8,8,8,9,9,9,9,9,9,10,11,13,16,20,20,20],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -4809,11 +4901,26 @@
       <c r="Z4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="AA4">
+        <v>20</v>
+      </c>
+      <c r="AB4">
+        <v>20</v>
+      </c>
+      <c r="AC4">
+        <v>20</v>
+      </c>
+      <c r="AD4">
+        <v>20</v>
+      </c>
+      <c r="AE4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Charlotte' ,2,4,6,8,8,11,14,15,17,19,20,20,22,23,23,24,24,24,26,29,29,33],</v>
+        <v>['Jeff', 'Charlotte' ,2,4,6,8,8,11,14,15,17,19,20,20,22,23,23,24,24,24,26,29,29,33,36,36,36],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -4888,11 +4995,26 @@
       <c r="Z5">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AA5">
+        <v>36</v>
+      </c>
+      <c r="AB5">
+        <v>36</v>
+      </c>
+      <c r="AC5">
+        <v>36</v>
+      </c>
+      <c r="AD5">
+        <v>36</v>
+      </c>
+      <c r="AE5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Chicago' ,1,3,5,8,10,11,12,13,14,16,18,21,21,23,25,26,28,29,31,31,32,35],</v>
+        <v>['Greg', 'Chicago' ,1,3,5,8,10,11,12,13,14,16,18,21,21,23,25,26,28,29,31,31,32,35,41,43,43],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -4967,11 +5089,26 @@
       <c r="Z6">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="AA6">
+        <v>41</v>
+      </c>
+      <c r="AB6">
+        <v>43</v>
+      </c>
+      <c r="AC6">
+        <v>43</v>
+      </c>
+      <c r="AD6">
+        <v>43</v>
+      </c>
+      <c r="AE6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Cleveland' ,2,5,7,10,12,13,16,19,22,25,27,29,30,31,33,36,39,40,42,42,45,47],</v>
+        <v>['Tim', 'Cleveland' ,2,5,7,10,12,13,16,19,22,25,27,29,30,31,33,36,39,40,42,42,45,47,51,55,59],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
@@ -5046,11 +5183,20 @@
       <c r="Z7">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="AA7">
+        <v>51</v>
+      </c>
+      <c r="AB7">
+        <v>55</v>
+      </c>
+      <c r="AC7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Dallas' ,0,0,2,2,2,3,5,6,9,10,11,13,14,16,20,21,22,22,25,28,29,31],</v>
+        <v>['Tim', 'Dallas' ,0,0,2,2,2,3,5,6,9,10,11,13,14,16,20,21,22,22,25,28,29,31,33,33,33],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -5125,11 +5271,26 @@
       <c r="Z8">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="AA8">
+        <v>33</v>
+      </c>
+      <c r="AB8">
+        <v>33</v>
+      </c>
+      <c r="AC8">
+        <v>33</v>
+      </c>
+      <c r="AD8">
+        <v>33</v>
+      </c>
+      <c r="AE8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Denver' ,1,2,3,4,6,7,8,11,12,14,14,15,17,20,22,24,25,26,28,30,33,35],</v>
+        <v>['Tim', 'Denver' ,1,2,3,4,6,7,8,11,12,14,14,15,17,20,22,24,25,26,28,30,33,35,40,40,40],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -5204,11 +5365,26 @@
       <c r="Z9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="AA9">
+        <v>40</v>
+      </c>
+      <c r="AB9">
+        <v>40</v>
+      </c>
+      <c r="AC9">
+        <v>40</v>
+      </c>
+      <c r="AD9">
+        <v>40</v>
+      </c>
+      <c r="AE9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Detroit' ,1,3,4,6,8,11,13,14,14,15,17,19,20,21,23,25,27,28,29,32,33,34],</v>
+        <v>['Greg', 'Detroit' ,1,3,4,6,8,11,13,14,14,15,17,19,20,21,23,25,27,28,29,32,33,34,37,37,37],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -5283,11 +5459,26 @@
       <c r="Z10">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:26">
+      <c r="AA10">
+        <v>37</v>
+      </c>
+      <c r="AB10">
+        <v>37</v>
+      </c>
+      <c r="AC10">
+        <v>37</v>
+      </c>
+      <c r="AD10">
+        <v>37</v>
+      </c>
+      <c r="AE10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Golden State' ,1,4,7,9,14,16,20,24,27,29,31,34,37,39,43,45,47,48,50,52,54,59],</v>
+        <v>['Zach', 'Golden State' ,1,4,7,9,14,16,20,24,27,29,31,34,37,39,43,45,47,48,50,52,54,59,67,71,75],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
@@ -5362,11 +5553,20 @@
       <c r="Z11">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="AA11">
+        <v>67</v>
+      </c>
+      <c r="AB11">
+        <v>71</v>
+      </c>
+      <c r="AC11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Houston' ,1,3,5,7,10,13,16,21,22,26,29,32,33,35,37,39,40,41,43,45,47,51],</v>
+        <v>['Jeff', 'Houston' ,1,3,5,7,10,13,16,21,22,26,29,32,33,35,37,39,40,41,43,45,47,51,55,59,61],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
@@ -5441,11 +5641,26 @@
       <c r="Z12">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="AA12">
+        <v>55</v>
+      </c>
+      <c r="AB12">
+        <v>59</v>
+      </c>
+      <c r="AC12">
+        <v>61</v>
+      </c>
+      <c r="AD12">
+        <v>61</v>
+      </c>
+      <c r="AE12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Indiana' ,1,2,4,6,8,9,11,14,15,16,19,20,22,24,27,29,29,30,31,33,35,37],</v>
+        <v>['Tim', 'Indiana' ,1,2,4,6,8,9,11,14,15,16,19,20,22,24,27,29,29,30,31,33,35,37,42,42,42],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -5520,11 +5735,26 @@
       <c r="Z13">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="AA13">
+        <v>42</v>
+      </c>
+      <c r="AB13">
+        <v>42</v>
+      </c>
+      <c r="AC13">
+        <v>42</v>
+      </c>
+      <c r="AD13">
+        <v>42</v>
+      </c>
+      <c r="AE13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8,10,10,11,11,12,14,15,16,16,17,19,19,19,19,20,20,21],</v>
+        <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8,10,10,11,11,12,14,15,16,16,17,19,19,19,19,20,20,21,26,26,26],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
@@ -5599,11 +5829,26 @@
       <c r="Z14">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="AA14">
+        <v>26</v>
+      </c>
+      <c r="AB14">
+        <v>26</v>
+      </c>
+      <c r="AC14">
+        <v>26</v>
+      </c>
+      <c r="AD14">
+        <v>26</v>
+      </c>
+      <c r="AE14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'LA Clippers' ,1,4,8,11,14,16,16,20,22,22,25,28,29,30,31,32,35,35,36,39,40,44],</v>
+        <v>['Greg', 'LA Clippers' ,1,4,8,11,14,16,16,20,22,22,25,28,29,30,31,32,35,35,36,39,40,44,51,54,54],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -5678,11 +5923,26 @@
       <c r="Z15">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="AA15">
+        <v>51</v>
+      </c>
+      <c r="AB15">
+        <v>54</v>
+      </c>
+      <c r="AC15">
+        <v>54</v>
+      </c>
+      <c r="AD15">
+        <v>54</v>
+      </c>
+      <c r="AE15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Memphis' ,1,3,4,7,10,12,16,18,20,22,23,25,26,27,30,33,34,34,36,36,39,40],</v>
+        <v>['Tim', 'Memphis' ,1,3,4,7,10,12,16,18,20,22,23,25,26,27,30,33,34,34,36,36,39,40,43,45,45],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -5757,11 +6017,26 @@
       <c r="Z16">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:26">
+      <c r="AA16">
+        <v>43</v>
+      </c>
+      <c r="AB16">
+        <v>45</v>
+      </c>
+      <c r="AC16">
+        <v>45</v>
+      </c>
+      <c r="AD16">
+        <v>45</v>
+      </c>
+      <c r="AE16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Miami' ,1,2,2,3,5,7,7,9,10,10,11,11,13,17,20,24,25,26,28,31,34,35],</v>
+        <v>['Zach', 'Miami' ,1,2,2,3,5,7,7,9,10,10,11,11,13,17,20,24,25,26,28,31,34,35,41,41,41],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -5836,11 +6111,26 @@
       <c r="Z17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="AA17">
+        <v>41</v>
+      </c>
+      <c r="AB17">
+        <v>41</v>
+      </c>
+      <c r="AC17">
+        <v>41</v>
+      </c>
+      <c r="AD17">
+        <v>41</v>
+      </c>
+      <c r="AE17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Milwaukee' ,0,3,4,5,6,9,11,13,14,16,18,20,20,21,21,22,25,25,27,31,34,37],</v>
+        <v>['Greg', 'Milwaukee' ,0,3,4,5,6,9,11,13,14,16,18,20,20,21,21,22,25,25,27,31,34,37,42,44,44],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -5915,11 +6205,26 @@
       <c r="Z18">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="AA18">
+        <v>42</v>
+      </c>
+      <c r="AB18">
+        <v>44</v>
+      </c>
+      <c r="AC18">
+        <v>44</v>
+      </c>
+      <c r="AD18">
+        <v>44</v>
+      </c>
+      <c r="AE18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Minnesota' ,0,1,2,4,5,5,6,7,9,11,11,14,15,17,19,20,22,23,25,27,28,28],</v>
+        <v>['Jeff', 'Minnesota' ,0,1,2,4,5,5,6,7,9,11,11,14,15,17,19,20,22,23,25,27,28,28,31,31,31],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -5994,11 +6299,26 @@
       <c r="Z19">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="AA19">
+        <v>31</v>
+      </c>
+      <c r="AB19">
+        <v>31</v>
+      </c>
+      <c r="AC19">
+        <v>31</v>
+      </c>
+      <c r="AD19">
+        <v>31</v>
+      </c>
+      <c r="AE19">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New Orleans' ,0,0,1,2,6,7,7,9,11,14,14,16,17,19,19,21,23,23,24,25,28,31],</v>
+        <v>['Zach', 'New Orleans' ,0,0,1,2,6,7,7,9,11,14,14,16,17,19,19,21,23,23,24,25,28,31,34,34,34],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -6073,11 +6393,26 @@
       <c r="Z20">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="AA20">
+        <v>34</v>
+      </c>
+      <c r="AB20">
+        <v>34</v>
+      </c>
+      <c r="AC20">
+        <v>34</v>
+      </c>
+      <c r="AD20">
+        <v>34</v>
+      </c>
+      <c r="AE20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'New York' ,0,2,3,5,8,10,13,14,16,16,17,18,19,21,22,22,23,23,25,26,27,27],</v>
+        <v>['Zach', 'New York' ,0,2,3,5,8,10,13,14,16,16,17,18,19,21,22,22,23,23,25,26,27,27,31,31,31],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -6152,11 +6487,26 @@
       <c r="Z21">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:26">
+      <c r="AA21">
+        <v>31</v>
+      </c>
+      <c r="AB21">
+        <v>31</v>
+      </c>
+      <c r="AC21">
+        <v>31</v>
+      </c>
+      <c r="AD21">
+        <v>31</v>
+      </c>
+      <c r="AE21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9,12,14,16,18,21,21,25,25,28,29,31,32,33,35,36,39,41],</v>
+        <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9,12,14,16,18,21,21,25,25,28,29,31,32,33,35,36,39,41,47,48,48],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
@@ -6231,11 +6581,26 @@
       <c r="Z22">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="AA22">
+        <v>47</v>
+      </c>
+      <c r="AB22">
+        <v>48</v>
+      </c>
+      <c r="AC22">
+        <v>48</v>
+      </c>
+      <c r="AD22">
+        <v>48</v>
+      </c>
+      <c r="AE22">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Orlando' ,0,2,3,5,6,8,10,12,14,15,16,17,18,18,20,20,21,21,23,24,25,27],</v>
+        <v>['Greg', 'Orlando' ,0,2,3,5,6,8,10,12,14,15,16,17,18,18,20,20,21,21,23,24,25,27,29,29,29],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
@@ -6310,11 +6675,26 @@
       <c r="Z23">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="AA23">
+        <v>29</v>
+      </c>
+      <c r="AB23">
+        <v>29</v>
+      </c>
+      <c r="AC23">
+        <v>29</v>
+      </c>
+      <c r="AD23">
+        <v>29</v>
+      </c>
+      <c r="AE23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Philadelphia' ,0,0,1,2,4,4,5,6,7,8,9,12,15,17,18,19,21,22,23,23,25,27],</v>
+        <v>['', 'Philadelphia' ,0,0,1,2,4,4,5,6,7,8,9,12,15,17,18,19,21,22,23,23,25,27,28,28,28],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="D24" t="s">
@@ -6386,11 +6766,26 @@
       <c r="Z24">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:26">
+      <c r="AA24">
+        <v>28</v>
+      </c>
+      <c r="AB24">
+        <v>28</v>
+      </c>
+      <c r="AC24">
+        <v>28</v>
+      </c>
+      <c r="AD24">
+        <v>28</v>
+      </c>
+      <c r="AE24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['', 'Phoenix' ,0,2,3,3,5,6,7,8,9,10,12,13,13,15,16,17,18,18,20,21,22,22],</v>
+        <v>['', 'Phoenix' ,0,2,3,3,5,6,7,8,9,10,12,13,13,15,16,17,18,18,20,21,22,22,24,24,24],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="D25" t="s">
@@ -6462,11 +6857,26 @@
       <c r="Z25">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:26">
+      <c r="AA25">
+        <v>24</v>
+      </c>
+      <c r="AB25">
+        <v>24</v>
+      </c>
+      <c r="AC25">
+        <v>24</v>
+      </c>
+      <c r="AD25">
+        <v>24</v>
+      </c>
+      <c r="AE25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Portland' ,1,3,6,7,9,10,12,13,13,14,16,18,18,21,22,23,23,24,25,28,30,35],</v>
+        <v>['Greg', 'Portland' ,1,3,6,7,9,10,12,13,13,14,16,18,18,21,22,23,23,24,25,28,30,35,41,41,41],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -6541,11 +6951,26 @@
       <c r="Z26">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="AA26">
+        <v>41</v>
+      </c>
+      <c r="AB26">
+        <v>41</v>
+      </c>
+      <c r="AC26">
+        <v>41</v>
+      </c>
+      <c r="AD26">
+        <v>41</v>
+      </c>
+      <c r="AE26">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'Sacramento' ,1,2,4,4,6,7,8,10,13,14,15,16,16,18,19,22,24,25,25,25,27,28],</v>
+        <v>['Jeff', 'Sacramento' ,1,2,4,4,6,7,8,10,13,14,15,16,16,18,19,22,24,25,25,25,27,28,32,32,32],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -6620,11 +7045,26 @@
       <c r="Z27">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:26">
+      <c r="AA27">
+        <v>32</v>
+      </c>
+      <c r="AB27">
+        <v>32</v>
+      </c>
+      <c r="AC27">
+        <v>32</v>
+      </c>
+      <c r="AD27">
+        <v>32</v>
+      </c>
+      <c r="AE27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Jeff', 'San Antonio' ,2,5,6,10,13,16,18,21,24,27,29,31,33,36,38,41,43,44,47,50,52,56],</v>
+        <v>['Jeff', 'San Antonio' ,2,5,6,10,13,16,18,21,24,27,29,31,33,36,38,41,43,44,47,50,52,56,61,65,69],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -6699,11 +7139,20 @@
       <c r="Z28">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:26">
+      <c r="AA28">
+        <v>61</v>
+      </c>
+      <c r="AB28">
+        <v>65</v>
+      </c>
+      <c r="AC28">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Greg', 'Toronto' ,1,4,6,8,10,13,16,18,21,22,24,27,28,29,30,32,33,34,37,38,40,44],</v>
+        <v>['Greg', 'Toronto' ,1,4,6,8,10,13,16,18,21,22,24,27,28,29,30,32,33,34,37,38,40,44,51,55,55],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -6778,11 +7227,26 @@
       <c r="Z29">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:26">
+      <c r="AA29">
+        <v>51</v>
+      </c>
+      <c r="AB29">
+        <v>55</v>
+      </c>
+      <c r="AC29">
+        <v>55</v>
+      </c>
+      <c r="AD29">
+        <v>55</v>
+      </c>
+      <c r="AE29">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Zach', 'Utah' ,1,3,6,7,9,11,14,17,18,21,22,26,28,30,31,34,35,36,38,41,43,44],</v>
+        <v>['Zach', 'Utah' ,1,3,6,7,9,11,14,17,18,21,22,26,28,30,31,34,35,36,38,41,43,44,51,55,55],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -6857,11 +7321,26 @@
       <c r="Z30">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:26">
+      <c r="AA30">
+        <v>51</v>
+      </c>
+      <c r="AB30">
+        <v>55</v>
+      </c>
+      <c r="AC30">
+        <v>55</v>
+      </c>
+      <c r="AD30">
+        <v>55</v>
+      </c>
+      <c r="AE30">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>['Tim', 'Washington' ,0,1,2,3,5,6,8,11,13,16,17,20,23,26,29,32,34,34,36,40,42,45],</v>
+        <v>['Tim', 'Washington' ,0,1,2,3,5,6,8,11,13,16,17,20,23,26,29,32,34,34,36,40,42,45,49,53,56],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -6936,18 +7415,33 @@
       <c r="Z31">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="AA31">
+        <v>49</v>
+      </c>
+      <c r="AB31">
+        <v>53</v>
+      </c>
+      <c r="AC31">
+        <v>56</v>
+      </c>
+      <c r="AD31">
+        <v>56</v>
+      </c>
+      <c r="AE31">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" s="4" customFormat="1" ht="4" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="4:26">
+    <row r="33" spans="4:29">
       <c r="D33" t="s">
         <v>32</v>
       </c>
       <c r="E33">
-        <f t="shared" ref="E33:Z35" si="2">SUMIF($C$2:$C$31,$D33,E$2:E$31)</f>
+        <f t="shared" ref="E33:AC35" si="2">SUMIF($C$2:$C$31,$D33,E$2:E$31)</f>
         <v>9</v>
       </c>
       <c r="F33" s="2">
@@ -7034,8 +7528,20 @@
         <f t="shared" si="2"/>
         <v>285</v>
       </c>
-    </row>
-    <row r="34" spans="4:26">
+      <c r="AA33" s="2">
+        <f t="shared" si="2"/>
+        <v>315</v>
+      </c>
+      <c r="AB33" s="2">
+        <f t="shared" si="2"/>
+        <v>328</v>
+      </c>
+      <c r="AC33" s="2">
+        <f t="shared" si="2"/>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="4:29">
       <c r="D34" t="s">
         <v>33</v>
       </c>
@@ -7127,8 +7633,20 @@
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="35" spans="4:26">
+      <c r="AA34" s="2">
+        <f t="shared" si="2"/>
+        <v>292</v>
+      </c>
+      <c r="AB34" s="2">
+        <f t="shared" si="2"/>
+        <v>303</v>
+      </c>
+      <c r="AC34" s="2">
+        <f t="shared" si="2"/>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="4:29">
       <c r="D35" t="s">
         <v>34</v>
       </c>
@@ -7220,13 +7738,25 @@
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="36" spans="4:26">
+      <c r="AA35" s="2">
+        <f t="shared" si="2"/>
+        <v>284</v>
+      </c>
+      <c r="AB35" s="2">
+        <f t="shared" si="2"/>
+        <v>294</v>
+      </c>
+      <c r="AC35" s="2">
+        <f t="shared" si="2"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="4:29">
       <c r="D36" t="s">
         <v>35</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:Z36" si="3">SUMIF($C$2:$C$31,$D$36,E$2:E$31)</f>
+        <f t="shared" ref="E36:AC36" si="3">SUMIF($C$2:$C$31,$D$36,E$2:E$31)</f>
         <v>5</v>
       </c>
       <c r="F36" s="2">
@@ -7312,6 +7842,18 @@
       <c r="Z36" s="2">
         <f t="shared" si="3"/>
         <v>249</v>
+      </c>
+      <c r="AA36" s="2">
+        <f t="shared" si="3"/>
+        <v>287</v>
+      </c>
+      <c r="AB36" s="2">
+        <f t="shared" si="3"/>
+        <v>297</v>
+      </c>
+      <c r="AC36" s="2">
+        <f t="shared" si="3"/>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to the 2017 NFL draft.
</commit_message>
<xml_diff>
--- a/Win Formatting.xlsx
+++ b/Win Formatting.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmiller/src/nfl_wins_league/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11660" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="11660" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -14,8 +19,11 @@
   <definedNames>
     <definedName name="teams" localSheetId="0">Original!$A$2:$G$9</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -39,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
   <si>
     <t>Arizona Cardinals</t>
   </si>
@@ -420,6 +428,12 @@
   </si>
   <si>
     <t>Finals</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Undrafted</t>
   </si>
 </sst>
 </file>
@@ -974,6 +988,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1309,7 +1328,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -1321,7 +1340,7 @@
     <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1347,7 +1366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1399,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1425,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1451,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1477,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1503,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1529,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1555,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10">
         <f>SUM(B2:B9)</f>
         <v>7</v>
@@ -1576,26 +1595,21 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="W6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="U11" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X17" sqref="X17"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="0.6640625" style="4" customWidth="1"/>
@@ -1610,36 +1624,16 @@
     <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
-      <c r="E1" s="7">
-        <f t="shared" ref="E1:I1" si="0">F1-7</f>
-        <v>42626</v>
-      </c>
-      <c r="F1" s="7">
-        <f t="shared" si="0"/>
-        <v>42633</v>
-      </c>
-      <c r="G1" s="7">
-        <f t="shared" si="0"/>
-        <v>42640</v>
-      </c>
-      <c r="H1" s="7">
-        <f t="shared" si="0"/>
-        <v>42647</v>
-      </c>
-      <c r="I1" s="7">
-        <f t="shared" si="0"/>
-        <v>42654</v>
-      </c>
-      <c r="J1" s="7">
-        <f>K1-7</f>
-        <v>42661</v>
-      </c>
-      <c r="K1" s="7">
-        <v>42668</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -1714,10 +1708,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>CONCATENATE("['",$C3,"', ","'",$D3,"', ",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,",",$U3,",",$V3,",",$W3,",",$X3,"],")</f>
-        <v>['Greg', '49ers', 1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,2,2,2,2,2],</v>
+        <f>CONCATENATE("['",$C3,"', ","'",$D3,"', ",$E3,"],")</f>
+        <v>['Greg', '49ers', 0],</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1727,73 +1721,14 @@
         <v>69</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>2</v>
-      </c>
-      <c r="X3">
-        <v>2</v>
-      </c>
-      <c r="Y3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A34" si="1">CONCATENATE("['",$C4,"', ","'",$D4,"', ",$E4,",",$F4,",",$G4,",",$H4,",",$I4,",",$J4,",",$K4,",",$L4,",",$M4,",",$N4,",",$O4,",",$P4,",",$Q4,",",$R4,",",$S4,",",$T4,",",$U4,",",$V4,",",$W4,",",$X4,"],")</f>
-        <v>['Jeff', 'Bears', 0,0,0,1,1,1,1,2,2,2,2,2,3,3,3,3,3,3,3,3],</v>
+        <f t="shared" ref="A4:A34" si="0">CONCATENATE("['",$C4,"', ","'",$D4,"', ",$E4,"],")</f>
+        <v>['Jeff', 'Bears', 0],</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -1805,71 +1740,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <v>3</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4">
-        <v>3</v>
-      </c>
-      <c r="U4">
-        <v>3</v>
-      </c>
-      <c r="V4">
-        <v>3</v>
-      </c>
-      <c r="W4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>3</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Bengals', 1,1,1,2,2,2,3,3,3,3,3,3,4,5,5,5,6,6,6,6],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Bengals', 0],</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -1879,73 +1755,14 @@
         <v>47</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
-        <v>3</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="Q5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>5</v>
-      </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-      <c r="U5">
-        <v>6</v>
-      </c>
-      <c r="V5">
-        <v>6</v>
-      </c>
-      <c r="W5">
-        <v>6</v>
-      </c>
-      <c r="X5">
-        <v>6</v>
-      </c>
-      <c r="Y5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Bills', 0,0,1,2,3,4,4,4,4,4,5,6,6,6,7,7,7,7,7,7],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Bills', 0],</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" t="s">
@@ -1957,151 +1774,33 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-      <c r="O6">
-        <v>5</v>
-      </c>
-      <c r="P6">
-        <v>6</v>
-      </c>
-      <c r="Q6">
-        <v>6</v>
-      </c>
-      <c r="R6">
-        <v>6</v>
-      </c>
-      <c r="S6">
-        <v>7</v>
-      </c>
-      <c r="T6">
-        <v>7</v>
-      </c>
-      <c r="U6">
-        <v>7</v>
-      </c>
-      <c r="V6">
-        <v>7</v>
-      </c>
-      <c r="W6">
-        <v>7</v>
-      </c>
-      <c r="X6">
-        <v>7</v>
-      </c>
-      <c r="Y6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Broncos', 1,2,3,4,4,4,5,6,6,7,7,7,8,8,8,8,9,9,9,9],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Broncos', 0],</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7">
-        <v>5</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-      <c r="M7">
-        <v>6</v>
-      </c>
-      <c r="N7">
-        <v>7</v>
-      </c>
-      <c r="O7">
-        <v>7</v>
-      </c>
-      <c r="P7">
-        <v>7</v>
-      </c>
-      <c r="Q7">
-        <v>8</v>
-      </c>
-      <c r="R7">
-        <v>8</v>
-      </c>
-      <c r="S7">
-        <v>8</v>
-      </c>
-      <c r="T7">
-        <v>8</v>
-      </c>
-      <c r="U7">
-        <v>9</v>
-      </c>
-      <c r="V7">
-        <v>9</v>
-      </c>
-      <c r="W7">
-        <v>9</v>
-      </c>
-      <c r="X7">
-        <v>9</v>
-      </c>
-      <c r="Y7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Browns', 0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,1,1,1,1,1],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Browns', 0],</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="D8" t="s">
         <v>49</v>
@@ -2109,151 +1808,33 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Buccaneers', 1,1,1,1,2,2,3,3,3,4,5,6,7,8,8,8,9,9,9,9],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Buccaneers', 0],</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>3</v>
-      </c>
-      <c r="M9">
-        <v>3</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>5</v>
-      </c>
-      <c r="P9">
-        <v>6</v>
-      </c>
-      <c r="Q9">
-        <v>7</v>
-      </c>
-      <c r="R9">
-        <v>8</v>
-      </c>
-      <c r="S9">
-        <v>8</v>
-      </c>
-      <c r="T9">
-        <v>8</v>
-      </c>
-      <c r="U9">
-        <v>9</v>
-      </c>
-      <c r="V9">
-        <v>9</v>
-      </c>
-      <c r="W9">
-        <v>9</v>
-      </c>
-      <c r="X9">
-        <v>9</v>
-      </c>
-      <c r="Y9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Cardinals', 0,1,1,1,2,3,3,3,3,4,4,4,5,5,5,6,7,7,7,7],</v>
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Cardinals', 0],</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>65</v>
@@ -2261,75 +1842,17 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="P10">
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <v>5</v>
-      </c>
-      <c r="R10">
-        <v>5</v>
-      </c>
-      <c r="S10" s="2">
-        <v>5</v>
-      </c>
-      <c r="T10">
-        <v>6</v>
-      </c>
-      <c r="U10">
-        <v>7</v>
-      </c>
-      <c r="V10">
-        <v>7</v>
-      </c>
-      <c r="W10">
-        <v>7</v>
-      </c>
-      <c r="X10">
-        <v>7</v>
-      </c>
-      <c r="Y10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="F10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Chargers', 0,1,1,1,1,2,3,3,4,4,4,5,5,5,5,5,5,5,5,5],</v>
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Chargers', 0],</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -2337,147 +1860,29 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
-      <c r="L11">
-        <v>3</v>
-      </c>
-      <c r="M11">
-        <v>4</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11">
-        <v>4</v>
-      </c>
-      <c r="P11">
-        <v>5</v>
-      </c>
-      <c r="Q11">
-        <v>5</v>
-      </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
-      <c r="S11">
-        <v>5</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-      <c r="U11">
-        <v>5</v>
-      </c>
-      <c r="V11">
-        <v>5</v>
-      </c>
-      <c r="W11">
-        <v>5</v>
-      </c>
-      <c r="X11">
-        <v>5</v>
-      </c>
-      <c r="Y11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Chiefs', 1,1,2,2,2,3,4,5,6,7,7,8,9,10,10,11,12,12,12,12],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Chiefs', 0],</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12">
-        <v>4</v>
-      </c>
-      <c r="L12">
-        <v>5</v>
-      </c>
-      <c r="M12">
-        <v>6</v>
-      </c>
-      <c r="N12">
-        <v>7</v>
-      </c>
-      <c r="O12">
-        <v>7</v>
-      </c>
-      <c r="P12">
-        <v>8</v>
-      </c>
-      <c r="Q12">
-        <v>9</v>
-      </c>
-      <c r="R12">
-        <v>10</v>
-      </c>
-      <c r="S12">
-        <v>10</v>
-      </c>
-      <c r="T12">
-        <v>11</v>
-      </c>
-      <c r="U12">
-        <v>12</v>
-      </c>
-      <c r="V12">
-        <v>12</v>
-      </c>
-      <c r="W12">
-        <v>12</v>
-      </c>
-      <c r="X12">
-        <v>12</v>
-      </c>
-      <c r="Y12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Colts', 0,0,1,1,2,2,3,3,4,4,5,5,6,6,7,7,8,8,8,8],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Colts', 0],</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
@@ -2489,75 +1894,16 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
-      <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>4</v>
-      </c>
-      <c r="N13">
-        <v>4</v>
-      </c>
-      <c r="O13">
-        <v>5</v>
-      </c>
-      <c r="P13">
-        <v>5</v>
-      </c>
-      <c r="Q13">
-        <v>6</v>
-      </c>
-      <c r="R13">
-        <v>6</v>
-      </c>
-      <c r="S13">
-        <v>7</v>
-      </c>
-      <c r="T13">
-        <v>7</v>
-      </c>
-      <c r="U13">
-        <v>8</v>
-      </c>
-      <c r="V13">
-        <v>8</v>
-      </c>
-      <c r="W13">
-        <v>8</v>
-      </c>
-      <c r="X13">
-        <v>8</v>
-      </c>
-      <c r="Y13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Cowboys', 0,1,2,3,4,5,5,6,7,8,9,10,11,11,12,13,13,13,13,13],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Cowboys', 0],</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
@@ -2565,75 +1911,16 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14">
-        <v>4</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
-      </c>
-      <c r="M14">
-        <v>7</v>
-      </c>
-      <c r="N14">
-        <v>8</v>
-      </c>
-      <c r="O14">
-        <v>9</v>
-      </c>
-      <c r="P14">
-        <v>10</v>
-      </c>
-      <c r="Q14">
-        <v>11</v>
-      </c>
-      <c r="R14">
-        <v>11</v>
-      </c>
-      <c r="S14">
-        <v>12</v>
-      </c>
-      <c r="T14">
-        <v>13</v>
-      </c>
-      <c r="U14">
-        <v>13</v>
-      </c>
-      <c r="V14">
-        <v>13</v>
-      </c>
-      <c r="W14">
-        <v>13</v>
-      </c>
-      <c r="X14">
-        <v>13</v>
-      </c>
-      <c r="Y14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Dolphins', 0,0,1,1,1,2,3,3,4,5,6,7,7,8,9,10,10,10,10,10],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Dolphins', 0],</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
         <v>58</v>
@@ -2641,147 +1928,29 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15">
-        <v>3</v>
-      </c>
-      <c r="M15">
-        <v>4</v>
-      </c>
-      <c r="N15">
-        <v>5</v>
-      </c>
-      <c r="O15">
-        <v>6</v>
-      </c>
-      <c r="P15">
-        <v>7</v>
-      </c>
-      <c r="Q15">
-        <v>7</v>
-      </c>
-      <c r="R15">
-        <v>8</v>
-      </c>
-      <c r="S15">
-        <v>9</v>
-      </c>
-      <c r="T15">
-        <v>10</v>
-      </c>
-      <c r="U15">
-        <v>10</v>
-      </c>
-      <c r="V15">
-        <v>10</v>
-      </c>
-      <c r="W15">
-        <v>10</v>
-      </c>
-      <c r="X15">
-        <v>10</v>
-      </c>
-      <c r="Y15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Eagles', 1,2,3,3,3,3,4,4,4,5,5,5,5,5,5,6,7,7,7,7],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Eagles', 0],</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>50</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
-      </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-      <c r="M16">
-        <v>4</v>
-      </c>
-      <c r="N16">
-        <v>5</v>
-      </c>
-      <c r="O16">
-        <v>5</v>
-      </c>
-      <c r="P16">
-        <v>5</v>
-      </c>
-      <c r="Q16">
-        <v>5</v>
-      </c>
-      <c r="R16">
-        <v>5</v>
-      </c>
-      <c r="S16">
-        <v>5</v>
-      </c>
-      <c r="T16">
-        <v>6</v>
-      </c>
-      <c r="U16">
-        <v>7</v>
-      </c>
-      <c r="V16">
-        <v>7</v>
-      </c>
-      <c r="W16">
-        <v>7</v>
-      </c>
-      <c r="X16">
-        <v>7</v>
-      </c>
-      <c r="Y16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Falcons', 0,1,2,3,4,4,4,5,6,6,6,7,7,8,9,10,11,11,12,13],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Falcons', 0],</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -2793,148 +1962,33 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>4</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
-      </c>
-      <c r="L17">
-        <v>5</v>
-      </c>
-      <c r="M17">
-        <v>6</v>
-      </c>
-      <c r="N17">
-        <v>6</v>
-      </c>
-      <c r="O17">
-        <v>6</v>
-      </c>
-      <c r="P17">
-        <v>7</v>
-      </c>
-      <c r="Q17">
-        <v>7</v>
-      </c>
-      <c r="R17">
-        <v>8</v>
-      </c>
-      <c r="S17">
-        <v>9</v>
-      </c>
-      <c r="T17">
-        <v>10</v>
-      </c>
-      <c r="U17">
-        <v>11</v>
-      </c>
-      <c r="V17">
-        <v>11</v>
-      </c>
-      <c r="W17">
-        <v>12</v>
-      </c>
-      <c r="X17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Giants', 1,2,2,2,2,3,4,4,5,6,7,8,8,9,10,10,11,11,11,11],</v>
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Giants', 0],</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>60</v>
       </c>
       <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>4</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <v>6</v>
-      </c>
-      <c r="O18">
-        <v>7</v>
-      </c>
-      <c r="P18">
-        <v>8</v>
-      </c>
-      <c r="Q18">
-        <v>8</v>
-      </c>
-      <c r="R18">
-        <v>9</v>
-      </c>
-      <c r="S18">
-        <v>10</v>
-      </c>
-      <c r="T18">
-        <v>10</v>
-      </c>
-      <c r="U18">
-        <v>11</v>
-      </c>
-      <c r="V18">
-        <v>11</v>
-      </c>
-      <c r="W18">
-        <v>11</v>
-      </c>
-      <c r="X18">
-        <v>11</v>
-      </c>
-      <c r="Y18">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Jaguars', 0,0,0,1,1,2,2,2,2,2,2,2,2,2,2,3,3,3,3,3],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Jaguars', 0],</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -2942,75 +1996,16 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <v>2</v>
-      </c>
-      <c r="M19">
-        <v>2</v>
-      </c>
-      <c r="N19">
-        <v>2</v>
-      </c>
-      <c r="O19">
-        <v>2</v>
-      </c>
-      <c r="P19">
-        <v>2</v>
-      </c>
-      <c r="Q19">
-        <v>2</v>
-      </c>
-      <c r="R19">
-        <v>2</v>
-      </c>
-      <c r="S19">
-        <v>2</v>
-      </c>
-      <c r="T19">
-        <v>3</v>
-      </c>
-      <c r="U19">
-        <v>3</v>
-      </c>
-      <c r="V19">
-        <v>3</v>
-      </c>
-      <c r="W19">
-        <v>3</v>
-      </c>
-      <c r="X19">
-        <v>3</v>
-      </c>
-      <c r="Y19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Jets', 0,1,1,1,1,1,2,3,3,3,3,3,3,4,4,4,5,5,5,5],</v>
+        <f t="shared" si="0"/>
+        <v>['Undrafted', 'Jets', 0],</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
@@ -3018,227 +2013,50 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>3</v>
-      </c>
-      <c r="M20">
-        <v>3</v>
-      </c>
-      <c r="N20">
-        <v>3</v>
-      </c>
-      <c r="O20">
-        <v>3</v>
-      </c>
-      <c r="P20">
-        <v>3</v>
-      </c>
-      <c r="Q20">
-        <v>3</v>
-      </c>
-      <c r="R20">
-        <v>4</v>
-      </c>
-      <c r="S20">
-        <v>4</v>
-      </c>
-      <c r="T20">
-        <v>4</v>
-      </c>
-      <c r="U20">
-        <v>5</v>
-      </c>
-      <c r="V20">
-        <v>5</v>
-      </c>
-      <c r="W20">
-        <v>5</v>
-      </c>
-      <c r="X20">
-        <v>5</v>
-      </c>
-      <c r="Y20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Lions', 1,1,1,1,2,3,4,4,5,5,6,7,8,9,9,9,9,9,9,9],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Lions', 0],</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
       </c>
       <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>3</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
-      </c>
-      <c r="L21">
-        <v>4</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="N21">
-        <v>5</v>
-      </c>
-      <c r="O21">
-        <v>6</v>
-      </c>
-      <c r="P21">
-        <v>7</v>
-      </c>
-      <c r="Q21">
-        <v>8</v>
-      </c>
-      <c r="R21">
-        <v>9</v>
-      </c>
-      <c r="S21">
-        <v>9</v>
-      </c>
-      <c r="T21">
-        <v>9</v>
-      </c>
-      <c r="U21">
-        <v>9</v>
-      </c>
-      <c r="V21">
-        <v>9</v>
-      </c>
-      <c r="W21">
-        <v>9</v>
-      </c>
-      <c r="X21">
-        <v>9</v>
-      </c>
-      <c r="Y21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Packers', 1,1,2,2,3,3,4,4,4,4,4,5,6,7,8,9,10,11,12,12],</v>
+        <f t="shared" si="0"/>
+        <v>['Greg', 'Packers', 0],</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
       <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>3</v>
-      </c>
-      <c r="J22">
-        <v>3</v>
-      </c>
-      <c r="K22">
-        <v>4</v>
-      </c>
-      <c r="L22">
-        <v>4</v>
-      </c>
-      <c r="M22">
-        <v>4</v>
-      </c>
-      <c r="N22">
-        <v>4</v>
-      </c>
-      <c r="O22">
-        <v>4</v>
-      </c>
-      <c r="P22">
-        <v>5</v>
-      </c>
-      <c r="Q22">
-        <v>6</v>
-      </c>
-      <c r="R22">
-        <v>7</v>
-      </c>
-      <c r="S22">
-        <v>8</v>
-      </c>
-      <c r="T22">
-        <v>9</v>
-      </c>
-      <c r="U22">
-        <v>10</v>
-      </c>
-      <c r="V22">
-        <v>11</v>
-      </c>
-      <c r="W22">
-        <v>12</v>
-      </c>
-      <c r="X22">
-        <v>12</v>
-      </c>
-      <c r="Y22">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Panthers', 0,1,1,1,1,1,1,2,3,3,4,4,4,5,6,6,6,6,6,6],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Panthers', 0],</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
         <v>39</v>
@@ -3246,224 +2064,50 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>2</v>
-      </c>
-      <c r="M23">
-        <v>3</v>
-      </c>
-      <c r="N23">
-        <v>3</v>
-      </c>
-      <c r="O23">
-        <v>4</v>
-      </c>
-      <c r="P23">
-        <v>4</v>
-      </c>
-      <c r="Q23">
-        <v>4</v>
-      </c>
-      <c r="R23">
-        <v>5</v>
-      </c>
-      <c r="S23">
-        <v>6</v>
-      </c>
-      <c r="T23">
-        <v>6</v>
-      </c>
-      <c r="U23">
-        <v>6</v>
-      </c>
-      <c r="V23">
-        <v>6</v>
-      </c>
-      <c r="W23">
-        <v>6</v>
-      </c>
-      <c r="X23">
-        <v>6</v>
-      </c>
-      <c r="Y23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Patriots', 1,2,3,3,4,5,6,7,7,7,8,9,10,11,12,13,14,14,15,16],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Patriots', 0],</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>64</v>
       </c>
       <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>4</v>
-      </c>
-      <c r="J24">
-        <v>5</v>
-      </c>
-      <c r="K24">
-        <v>6</v>
-      </c>
-      <c r="L24">
-        <v>7</v>
-      </c>
-      <c r="M24">
-        <v>7</v>
-      </c>
-      <c r="N24">
-        <v>7</v>
-      </c>
-      <c r="O24">
-        <v>8</v>
-      </c>
-      <c r="P24">
-        <v>9</v>
-      </c>
-      <c r="Q24">
-        <v>10</v>
-      </c>
-      <c r="R24">
-        <v>11</v>
-      </c>
-      <c r="S24">
-        <v>12</v>
-      </c>
-      <c r="T24">
-        <v>13</v>
-      </c>
-      <c r="U24">
-        <v>14</v>
-      </c>
-      <c r="V24">
-        <v>14</v>
-      </c>
-      <c r="W24">
-        <v>15</v>
-      </c>
-      <c r="X24">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Raiders', 1,1,2,3,4,4,5,6,7,7,8,9,10,10,11,12,12,12,12,12],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Raiders', 0],</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25">
-        <v>4</v>
-      </c>
-      <c r="J25">
-        <v>4</v>
-      </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
-      <c r="L25">
-        <v>6</v>
-      </c>
-      <c r="M25">
-        <v>7</v>
-      </c>
-      <c r="N25">
-        <v>7</v>
-      </c>
-      <c r="O25">
-        <v>8</v>
-      </c>
-      <c r="P25">
-        <v>9</v>
-      </c>
-      <c r="Q25">
-        <v>10</v>
-      </c>
-      <c r="R25">
-        <v>10</v>
-      </c>
-      <c r="S25">
-        <v>11</v>
-      </c>
-      <c r="T25">
-        <v>12</v>
-      </c>
-      <c r="U25">
-        <v>12</v>
-      </c>
-      <c r="V25">
-        <v>12</v>
-      </c>
-      <c r="W25">
-        <v>12</v>
-      </c>
-      <c r="X25">
-        <v>12</v>
-      </c>
-      <c r="Y25">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Rams', 0,1,2,3,3,3,3,3,3,4,4,4,4,4,4,4,4,4,4,4],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Rams', 0],</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>68</v>
@@ -3471,71 +2115,12 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26">
-        <v>3</v>
-      </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-      <c r="K26">
-        <v>3</v>
-      </c>
-      <c r="L26">
-        <v>3</v>
-      </c>
-      <c r="M26">
-        <v>3</v>
-      </c>
-      <c r="N26">
-        <v>4</v>
-      </c>
-      <c r="O26">
-        <v>4</v>
-      </c>
-      <c r="P26">
-        <v>4</v>
-      </c>
-      <c r="Q26">
-        <v>4</v>
-      </c>
-      <c r="R26">
-        <v>4</v>
-      </c>
-      <c r="S26">
-        <v>4</v>
-      </c>
-      <c r="T26">
-        <v>4</v>
-      </c>
-      <c r="U26">
-        <v>4</v>
-      </c>
-      <c r="V26">
-        <v>4</v>
-      </c>
-      <c r="W26">
-        <v>4</v>
-      </c>
-      <c r="X26">
-        <v>4</v>
-      </c>
-      <c r="Y26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Ravens', 1,2,3,3,3,3,3,3,4,5,5,6,7,7,8,8,8,8,8,8],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Ravens', 0],</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -3545,77 +2130,18 @@
         <v>55</v>
       </c>
       <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
-      </c>
-      <c r="J27">
-        <v>3</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>3</v>
-      </c>
-      <c r="M27">
-        <v>4</v>
-      </c>
-      <c r="N27">
-        <v>5</v>
-      </c>
-      <c r="O27">
-        <v>5</v>
-      </c>
-      <c r="P27">
-        <v>6</v>
-      </c>
-      <c r="Q27">
-        <v>7</v>
-      </c>
-      <c r="R27">
-        <v>7</v>
-      </c>
-      <c r="S27">
-        <v>8</v>
-      </c>
-      <c r="T27">
-        <v>8</v>
-      </c>
-      <c r="U27">
-        <v>8</v>
-      </c>
-      <c r="V27">
-        <v>8</v>
-      </c>
-      <c r="W27">
-        <v>8</v>
-      </c>
-      <c r="X27">
-        <v>8</v>
-      </c>
-      <c r="Y27">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Greg', 'Redskins', 0,0,1,2,3,4,4,4,4,5,6,6,6,7,7,8,8,8,8,8],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Redskins', 0],</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="D28" t="s">
         <v>67</v>
@@ -3623,71 +2149,12 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="I28">
-        <v>3</v>
-      </c>
-      <c r="J28">
-        <v>4</v>
-      </c>
-      <c r="K28">
-        <v>4</v>
-      </c>
-      <c r="L28">
-        <v>4</v>
-      </c>
-      <c r="M28">
-        <v>4</v>
-      </c>
-      <c r="N28">
-        <v>5</v>
-      </c>
-      <c r="O28">
-        <v>6</v>
-      </c>
-      <c r="P28">
-        <v>6</v>
-      </c>
-      <c r="Q28">
-        <v>6</v>
-      </c>
-      <c r="R28">
-        <v>7</v>
-      </c>
-      <c r="S28">
-        <v>7</v>
-      </c>
-      <c r="T28">
-        <v>8</v>
-      </c>
-      <c r="U28">
-        <v>8</v>
-      </c>
-      <c r="V28">
-        <v>8</v>
-      </c>
-      <c r="W28">
-        <v>8</v>
-      </c>
-      <c r="X28">
-        <v>8</v>
-      </c>
-      <c r="Y28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Saints', 0,0,0,1,1,2,2,3,4,4,4,5,5,5,6,7,7,7,7,7],</v>
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Saints', 0],</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -3699,223 +2166,46 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>2</v>
-      </c>
-      <c r="K29">
-        <v>2</v>
-      </c>
-      <c r="L29">
-        <v>3</v>
-      </c>
-      <c r="M29">
-        <v>4</v>
-      </c>
-      <c r="N29">
-        <v>4</v>
-      </c>
-      <c r="O29">
-        <v>4</v>
-      </c>
-      <c r="P29">
-        <v>5</v>
-      </c>
-      <c r="Q29">
-        <v>5</v>
-      </c>
-      <c r="R29">
-        <v>5</v>
-      </c>
-      <c r="S29">
-        <v>6</v>
-      </c>
-      <c r="T29">
-        <v>7</v>
-      </c>
-      <c r="U29">
-        <v>7</v>
-      </c>
-      <c r="V29">
-        <v>7</v>
-      </c>
-      <c r="W29">
-        <v>7</v>
-      </c>
-      <c r="X29">
-        <v>7</v>
-      </c>
-      <c r="Y29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Seahawks', 1,1,2,3,3,4,4,4,5,6,7,7,8,8,9,9,10,11,11,11],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Seahawks', 0],</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
         <v>59</v>
       </c>
       <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="J30">
-        <v>4</v>
-      </c>
-      <c r="K30">
-        <v>4</v>
-      </c>
-      <c r="L30">
-        <v>4</v>
-      </c>
-      <c r="M30">
-        <v>5</v>
-      </c>
-      <c r="N30">
-        <v>6</v>
-      </c>
-      <c r="O30">
-        <v>7</v>
-      </c>
-      <c r="P30">
-        <v>7</v>
-      </c>
-      <c r="Q30">
-        <v>8</v>
-      </c>
-      <c r="R30">
-        <v>8</v>
-      </c>
-      <c r="S30">
-        <v>9</v>
-      </c>
-      <c r="T30">
-        <v>9</v>
-      </c>
-      <c r="U30">
-        <v>10</v>
-      </c>
-      <c r="V30">
-        <v>11</v>
-      </c>
-      <c r="W30">
-        <v>11</v>
-      </c>
-      <c r="X30">
-        <v>11</v>
-      </c>
-      <c r="Y30">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Steelers', 1,2,2,3,4,4,4,4,4,4,5,6,7,8,9,10,11,12,13,13],</v>
+        <f t="shared" si="0"/>
+        <v>['Zach', 'Steelers', 0],</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
       </c>
       <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <v>2</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31">
-        <v>3</v>
-      </c>
-      <c r="I31">
-        <v>4</v>
-      </c>
-      <c r="J31">
-        <v>4</v>
-      </c>
-      <c r="K31">
-        <v>4</v>
-      </c>
-      <c r="L31">
-        <v>4</v>
-      </c>
-      <c r="M31">
-        <v>4</v>
-      </c>
-      <c r="N31">
-        <v>4</v>
-      </c>
-      <c r="O31">
-        <v>5</v>
-      </c>
-      <c r="P31">
-        <v>6</v>
-      </c>
-      <c r="Q31">
-        <v>7</v>
-      </c>
-      <c r="R31">
-        <v>8</v>
-      </c>
-      <c r="S31">
-        <v>9</v>
-      </c>
-      <c r="T31">
-        <v>10</v>
-      </c>
-      <c r="U31">
-        <v>11</v>
-      </c>
-      <c r="V31">
-        <v>12</v>
-      </c>
-      <c r="W31">
-        <v>13</v>
-      </c>
-      <c r="X31">
-        <v>13</v>
-      </c>
-      <c r="Y31">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Jeff', 'Texans', 1,2,2,3,3,4,4,5,5,6,6,6,6,7,8,9,9,10,10,10],</v>
+        <f t="shared" si="0"/>
+        <v>['Jeff', 'Texans', 0],</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -3925,77 +2215,18 @@
         <v>53</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
-        <v>2</v>
-      </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
-      <c r="H32">
-        <v>3</v>
-      </c>
-      <c r="I32">
-        <v>3</v>
-      </c>
-      <c r="J32">
-        <v>4</v>
-      </c>
-      <c r="K32">
-        <v>4</v>
-      </c>
-      <c r="L32">
-        <v>5</v>
-      </c>
-      <c r="M32">
-        <v>5</v>
-      </c>
-      <c r="N32">
-        <v>6</v>
-      </c>
-      <c r="O32">
-        <v>6</v>
-      </c>
-      <c r="P32">
-        <v>6</v>
-      </c>
-      <c r="Q32">
-        <v>6</v>
-      </c>
-      <c r="R32">
-        <v>7</v>
-      </c>
-      <c r="S32">
-        <v>8</v>
-      </c>
-      <c r="T32">
-        <v>9</v>
-      </c>
-      <c r="U32">
-        <v>9</v>
-      </c>
-      <c r="V32">
-        <v>10</v>
-      </c>
-      <c r="W32">
-        <v>10</v>
-      </c>
-      <c r="X32">
-        <v>10</v>
-      </c>
-      <c r="Y32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Zach', 'Titans', 0,1,1,1,2,3,3,4,4,5,5,6,6,7,8,8,9,9,9,9],</v>
+        <f t="shared" si="0"/>
+        <v>['Tim', 'Titans', 0],</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>51</v>
@@ -4003,75 +2234,16 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="J33">
-        <v>3</v>
-      </c>
-      <c r="K33">
-        <v>3</v>
-      </c>
-      <c r="L33">
-        <v>4</v>
-      </c>
-      <c r="M33">
-        <v>4</v>
-      </c>
-      <c r="N33">
-        <v>5</v>
-      </c>
-      <c r="O33">
-        <v>5</v>
-      </c>
-      <c r="P33">
-        <v>6</v>
-      </c>
-      <c r="Q33">
-        <v>6</v>
-      </c>
-      <c r="R33">
-        <v>7</v>
-      </c>
-      <c r="S33">
-        <v>8</v>
-      </c>
-      <c r="T33">
-        <v>8</v>
-      </c>
-      <c r="U33">
-        <v>9</v>
-      </c>
-      <c r="V33">
-        <v>9</v>
-      </c>
-      <c r="W33">
-        <v>9</v>
-      </c>
-      <c r="X33">
-        <v>9</v>
-      </c>
-      <c r="Y33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>['Tim', 'Vikings', 1,2,3,4,5,5,5,5,5,5,6,6,6,7,7,7,8,8,8,8],</v>
+        <f t="shared" si="0"/>
+        <v>['Mike', 'Vikings', 1],</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="D34" t="s">
         <v>74</v>
@@ -4079,426 +2251,456 @@
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34" s="2">
-        <v>2</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-      <c r="H34">
-        <v>4</v>
-      </c>
-      <c r="I34">
-        <v>5</v>
-      </c>
-      <c r="J34">
-        <v>5</v>
-      </c>
-      <c r="K34">
-        <v>5</v>
-      </c>
-      <c r="L34">
-        <v>5</v>
-      </c>
-      <c r="M34">
-        <v>5</v>
-      </c>
-      <c r="N34">
-        <v>5</v>
-      </c>
-      <c r="O34">
-        <v>6</v>
-      </c>
-      <c r="P34">
-        <v>6</v>
-      </c>
-      <c r="Q34">
-        <v>6</v>
-      </c>
-      <c r="R34">
-        <v>7</v>
-      </c>
-      <c r="S34">
-        <v>7</v>
-      </c>
-      <c r="T34">
-        <v>7</v>
-      </c>
-      <c r="U34">
-        <v>8</v>
-      </c>
-      <c r="V34">
-        <v>8</v>
-      </c>
-      <c r="W34">
-        <v>8</v>
-      </c>
-      <c r="X34">
-        <v>8</v>
-      </c>
-      <c r="Y34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" s="4" customFormat="1" ht="4" customHeight="1">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:25" s="4" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>32</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36:U38" si="2">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
-        <v>4</v>
+        <f t="shared" ref="E36:U38" si="1">SUMIF($C$3:$C$34,$D36,E$3:E$34)</f>
+        <v>0</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="2"/>
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Q36" s="2">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R36" s="2">
-        <f t="shared" si="2"/>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="S36" s="2">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T36" s="2">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="U36" s="2">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="V36" s="2">
-        <f t="shared" ref="U36:Y38" si="3">SUMIF($C$3:$C$34,$D36,V$3:V$34)</f>
-        <v>54</v>
+        <f t="shared" ref="U36:Y38" si="2">SUMIF($C$3:$C$34,$D36,V$3:V$34)</f>
+        <v>0</v>
       </c>
       <c r="W36" s="2">
-        <f t="shared" si="3"/>
-        <v>54</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="X36" s="2">
-        <f t="shared" si="3"/>
-        <v>54</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="Y36" s="2">
-        <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>33</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="2"/>
-        <v>38</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" si="2"/>
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Q37" s="2">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R37" s="2">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="S37" s="2">
-        <f t="shared" si="2"/>
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T37" s="2">
-        <f t="shared" si="2"/>
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="U37" s="2">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="V37" s="2">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="W37" s="2">
-        <f t="shared" si="3"/>
-        <v>71</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="X37" s="2">
-        <f t="shared" si="3"/>
-        <v>73</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="Y37" s="2">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>34</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="2"/>
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Q38" s="2">
-        <f t="shared" si="2"/>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="R38" s="2">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="S38" s="2">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="T38" s="2">
-        <f t="shared" si="2"/>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="U38" s="2">
-        <f t="shared" si="3"/>
-        <v>65</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="V38" s="2">
-        <f t="shared" si="3"/>
-        <v>67</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="W38" s="2">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="X38" s="2">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="Y38" s="2">
-        <f t="shared" si="3"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>35</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:Y39" si="4">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
-        <v>5</v>
+        <f t="shared" ref="E39:Y40" si="3">SUMIF($C$3:$C$34,$D$39,E$3:E$34)</f>
+        <v>0</v>
       </c>
       <c r="F39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40">
+        <f>SUMIF($C$3:$C$34,$D$40,E$3:E$34)</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>SUMIF($C$3:$C$34,$D$40,F$3:F$34)</f>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:Y40" si="4">SUMIF($C$3:$C$34,$D$40,G$3:G$34)</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="J39" s="2">
+        <v>0</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="L39" s="2">
+        <v>0</v>
+      </c>
+      <c r="N40">
         <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="M39" s="2">
+        <v>0</v>
+      </c>
+      <c r="O40">
         <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="N39" s="2">
+        <v>0</v>
+      </c>
+      <c r="P40">
         <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="O39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q40">
         <f t="shared" si="4"/>
-        <v>44</v>
-      </c>
-      <c r="P39" s="2">
+        <v>0</v>
+      </c>
+      <c r="R40">
         <f t="shared" si="4"/>
-        <v>48</v>
-      </c>
-      <c r="Q39" s="2">
+        <v>0</v>
+      </c>
+      <c r="S40">
         <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="R39" s="2">
+        <v>0</v>
+      </c>
+      <c r="T40">
         <f t="shared" si="4"/>
-        <v>55</v>
-      </c>
-      <c r="S39" s="2">
+        <v>0</v>
+      </c>
+      <c r="U40">
         <f t="shared" si="4"/>
-        <v>58</v>
-      </c>
-      <c r="T39" s="2">
+        <v>0</v>
+      </c>
+      <c r="V40">
         <f t="shared" si="4"/>
-        <v>61</v>
-      </c>
-      <c r="U39" s="2">
+        <v>0</v>
+      </c>
+      <c r="W40">
         <f t="shared" si="4"/>
-        <v>67</v>
-      </c>
-      <c r="V39" s="2">
+        <v>0</v>
+      </c>
+      <c r="X40">
         <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-      <c r="W39" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y40">
         <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-      <c r="X39" s="2">
-        <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-      <c r="Y39" s="2">
-        <f t="shared" si="4"/>
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4507,11 +2709,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4519,12 +2716,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AA1" activePane="topRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="0.6640625" style="4" customWidth="1"/>
@@ -4534,7 +2731,7 @@
     <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -4641,7 +2838,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
         <f>CONCATENATE("['",$C2,"', ","'",$D2,"' ,",$E2,",",$F2,",",$G2,",",$H2,",",$I2,",",$J2,",",$K2,",",$L2,",",$M2,",",$N2,",",$O2,",",$P2,",",$Q2,",",$R2,",",$S2,",",$T2,",",$U2,",",$V2,",",$W2,",",$X2,",",$Y2,",",$Z2,",",$AA2,",",$AB2,",",$AC2,"],")</f>
         <v>['Zach', 'Atlanta' ,1,3,6,9,10,10,12,13,15,17,20,23,25,27,29,31,32,32,34,36,37,37,43,45,45],</v>
@@ -4735,7 +2932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
         <f t="shared" ref="A3:A31" si="1">CONCATENATE("['",$C3,"', ","'",$D3,"' ,",$E3,",",$F3,",",$G3,",",$H3,",",$I3,",",$J3,",",$K3,",",$L3,",",$M3,",",$N3,",",$O3,",",$P3,",",$Q3,",",$R3,",",$S3,",",$T3,",",$U3,",",$V3,",",$W3,",",$X3,",",$Y3,",",$Z3,",",$AA3,",",$AB3,",",$AC3,"],")</f>
         <v>['Jeff', 'Boston' ,1,3,4,6,9,11,13,14,17,20,22,25,26,28,32,34,37,37,40,41,44,48,53,57,61],</v>
@@ -4823,7 +3020,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'Brooklyn' ,1,2,3,4,4,5,6,7,7,8,8,8,9,9,9,9,9,9,10,11,13,16,20,20,20],</v>
@@ -4917,7 +3114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'Charlotte' ,2,4,6,8,8,11,14,15,17,19,20,20,22,23,23,24,24,24,26,29,29,33,36,36,36],</v>
@@ -5011,7 +3208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Chicago' ,1,3,5,8,10,11,12,13,14,16,18,21,21,23,25,26,28,29,31,31,32,35,41,43,43],</v>
@@ -5105,7 +3302,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Cleveland' ,2,5,7,10,12,13,16,19,22,25,27,29,30,31,33,36,39,40,42,42,45,47,51,55,59],</v>
@@ -5193,7 +3390,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Dallas' ,0,0,2,2,2,3,5,6,9,10,11,13,14,16,20,21,22,22,25,28,29,31,33,33,33],</v>
@@ -5287,7 +3484,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Denver' ,1,2,3,4,6,7,8,11,12,14,14,15,17,20,22,24,25,26,28,30,33,35,40,40,40],</v>
@@ -5381,7 +3578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Detroit' ,1,3,4,6,8,11,13,14,14,15,17,19,20,21,23,25,27,28,29,32,33,34,37,37,37],</v>
@@ -5475,7 +3672,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'Golden State' ,1,4,7,9,14,16,20,24,27,29,31,34,37,39,43,45,47,48,50,52,54,59,67,71,75],</v>
@@ -5563,7 +3760,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'Houston' ,1,3,5,7,10,13,16,21,22,26,29,32,33,35,37,39,40,41,43,45,47,51,55,59,61],</v>
@@ -5657,7 +3854,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Indiana' ,1,2,4,6,8,9,11,14,15,16,19,20,22,24,27,29,29,30,31,33,35,37,42,42,42],</v>
@@ -5751,7 +3948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'L.A. Lakers' ,1,3,5,7,8,10,10,11,11,12,14,15,16,16,17,19,19,19,19,20,20,21,26,26,26],</v>
@@ -5845,7 +4042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'LA Clippers' ,1,4,8,11,14,16,16,20,22,22,25,28,29,30,31,32,35,35,36,39,40,44,51,54,54],</v>
@@ -5939,7 +4136,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Memphis' ,1,3,4,7,10,12,16,18,20,22,23,25,26,27,30,33,34,34,36,36,39,40,43,45,45],</v>
@@ -6033,7 +4230,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'Miami' ,1,2,2,3,5,7,7,9,10,10,11,11,13,17,20,24,25,26,28,31,34,35,41,41,41],</v>
@@ -6127,7 +4324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Milwaukee' ,0,3,4,5,6,9,11,13,14,16,18,20,20,21,21,22,25,25,27,31,34,37,42,44,44],</v>
@@ -6221,7 +4418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'Minnesota' ,0,1,2,4,5,5,6,7,9,11,11,14,15,17,19,20,22,23,25,27,28,28,31,31,31],</v>
@@ -6315,7 +4512,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'New Orleans' ,0,0,1,2,6,7,7,9,11,14,14,16,17,19,19,21,23,23,24,25,28,31,34,34,34],</v>
@@ -6409,7 +4606,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'New York' ,0,2,3,5,8,10,13,14,16,16,17,18,19,21,22,22,23,23,25,26,27,27,31,31,31],</v>
@@ -6503,7 +4700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'Oklahoma City' ,2,4,6,7,9,12,14,16,18,21,21,25,25,28,29,31,32,33,35,36,39,41,47,48,48],</v>
@@ -6597,7 +4794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Orlando' ,0,2,3,5,6,8,10,12,14,15,16,17,18,18,20,20,21,21,23,24,25,27,29,29,29],</v>
@@ -6691,7 +4888,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['', 'Philadelphia' ,0,0,1,2,4,4,5,6,7,8,9,12,15,17,18,19,21,22,23,23,25,27,28,28,28],</v>
@@ -6782,7 +4979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['', 'Phoenix' ,0,2,3,3,5,6,7,8,9,10,12,13,13,15,16,17,18,18,20,21,22,22,24,24,24],</v>
@@ -6873,7 +5070,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Portland' ,1,3,6,7,9,10,12,13,13,14,16,18,18,21,22,23,23,24,25,28,30,35,41,41,41],</v>
@@ -6967,7 +5164,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'Sacramento' ,1,2,4,4,6,7,8,10,13,14,15,16,16,18,19,22,24,25,25,25,27,28,32,32,32],</v>
@@ -7061,7 +5258,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Jeff', 'San Antonio' ,2,5,6,10,13,16,18,21,24,27,29,31,33,36,38,41,43,44,47,50,52,56,61,65,69],</v>
@@ -7149,7 +5346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Greg', 'Toronto' ,1,4,6,8,10,13,16,18,21,22,24,27,28,29,30,32,33,34,37,38,40,44,51,55,55],</v>
@@ -7243,7 +5440,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Zach', 'Utah' ,1,3,6,7,9,11,14,17,18,21,22,26,28,30,31,34,35,36,38,41,43,44,51,55,55],</v>
@@ -7337,7 +5534,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
         <f t="shared" si="1"/>
         <v>['Tim', 'Washington' ,0,1,2,3,5,6,8,11,13,16,17,20,23,26,29,32,34,34,36,40,42,45,49,53,56],</v>
@@ -7431,12 +5628,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:31" s="4" customFormat="1" ht="4" customHeight="1">
+    <row r="32" spans="1:31" s="4" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="4:29">
+    <row r="33" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>32</v>
       </c>
@@ -7541,7 +5738,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="34" spans="4:29">
+    <row r="34" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>33</v>
       </c>
@@ -7646,7 +5843,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="35" spans="4:29">
+    <row r="35" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>34</v>
       </c>
@@ -7751,7 +5948,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="4:29">
+    <row r="36" spans="4:29" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>35</v>
       </c>
@@ -7859,10 +6056,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>